<commit_message>
fix: redoing the filtering
</commit_message>
<xml_diff>
--- a/llm_filtered_jobs.xlsx
+++ b/llm_filtered_jobs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>run_id</t>
   </si>
@@ -73,7 +73,13 @@
     <t>Video Testimonial Editor Clean-Up Task - Upwork</t>
   </si>
   <si>
+    <t>Seeking DaVinci Resolve Mentor/Trainer for YouTube/IG Video Editing - Upwork</t>
+  </si>
+  <si>
     <t>https://www.upwork.com/jobs/Video-Testimonial-Editor-Clean-Task_%7E0122433972068704d4?source=rss</t>
+  </si>
+  <si>
+    <t>https://www.upwork.com/jobs/Seeking-DaVinci-Resolve-Mentor-Trainer-for-YouTube-Video-Editing_%7E0156e8d9b16867f12d?source=rss</t>
   </si>
   <si>
     <t xml:space="preserve">Task Overview
@@ -113,6 +119,36 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">I am looking for someone who can help me learn to use DaVinci Resolve in order to do some video editing tasks I need to regularly complete for two YouTube channels. 
+I have some experience with DaVinci Resolve, but I've forgotten a lot, and I could use some help. 
+The way in which I'd like to work together is that we meet by Zoom for 15-30 hours total over the next month or so, and we work on editing actual footage I have for two YouTube channels.
+Channel 1: Mostly talking head style footage with some B-Roll
+Channel 2: Mix of talking head style footage and travel vlog footage.
+There are several tasks I need help with. Some of these tasks are one-off tasks, and other tasks are repeated tasks.
+One off tasks
+- Create a channel intro
+- Create an in-video &amp;quot;Chapter&amp;quot; transition
+Repeated task
+- Edit out parts of the video where I misspeak
+- Find and add b-roll footage/images
+- Color grade
+- Find and add appropriate music/sound effects (I have an Epidemic Sounds subscription)
+Hourly Range
+: $12.00-$36.00
+Posted On
+: June 14, 2024 21:18 UTC
+Category
+: Video Editing
+Skills
+:DaVinci Resolve,     Video Post-Editing    
+Skills
+:        DaVinci Resolve,                     Video Post-Editing            
+Country
+: United States
+click to apply
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Task Overview&lt;br /&gt;
 We are looking for skilled video editors to help clean up and enhance testimonial videos. The primary focus is on removing dead space, adding live captions, and ensuring the overall quality of the video is high. This description outlines the details and requirements for the task.&lt;br /&gt;&lt;br /&gt;
 Candidate Requirements&lt;br /&gt;
@@ -140,19 +176,51 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">I am looking for someone who can help me learn to use DaVinci Resolve in order to do some video editing tasks I need to regularly complete for two YouTube channels. &lt;br /&gt;&lt;br /&gt;
+I have some experience with DaVinci Resolve, but I&amp;#039;ve forgotten a lot, and I could use some help. &lt;br /&gt;&lt;br /&gt;
+The way in which I&amp;#039;d like to work together is that we meet by Zoom for 15-30 hours total over the next month or so, and we work on editing actual footage I have for two YouTube channels.&lt;br /&gt;&lt;br /&gt;
+Channel 1: Mostly talking head style footage with some B-Roll&lt;br /&gt;
+Channel 2: Mix of talking head style footage and travel vlog footage.&lt;br /&gt;&lt;br /&gt;
+There are several tasks I need help with. Some of these tasks are one-off tasks, and other tasks are repeated tasks.&lt;br /&gt;&lt;br /&gt;
+One off tasks&lt;br /&gt;
+- Create a channel intro&lt;br /&gt;
+- Create an in-video &amp;amp;quot;Chapter&amp;amp;quot; transition&lt;br /&gt;&lt;br /&gt;
+Repeated task&lt;br /&gt;
+- Edit out parts of the video where I misspeak&lt;br /&gt;
+- Find and add b-roll footage/images&lt;br /&gt;
+- Color grade&lt;br /&gt;
+- Find and add appropriate music/sound effects (I have an Epidemic Sounds subscription)&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Hourly Range&lt;/b&gt;: $12.00-$36.00
+&lt;br /&gt;&lt;b&gt;Posted On&lt;/b&gt;: June 14, 2024 21:18 UTC&lt;br /&gt;&lt;b&gt;Category&lt;/b&gt;: Video Editing&lt;br /&gt;&lt;b&gt;Skills&lt;/b&gt;:DaVinci Resolve,     Video Post-Editing    
+&lt;br /&gt;&lt;b&gt;Skills&lt;/b&gt;:        DaVinci Resolve,                     Video Post-Editing            &lt;br /&gt;&lt;b&gt;Country&lt;/b&gt;: United States
+&lt;br /&gt;&lt;a href="https://www.upwork.com/jobs/Seeking-DaVinci-Resolve-Mentor-Trainer-for-YouTube-Video-Editing_%7E0156e8d9b16867f12d?source=rss"&gt;click to apply&lt;/a&gt;
+</t>
+  </si>
+  <si>
     <t>Fri, 14 Jun 2024 21:50:28 +0000</t>
   </si>
   <si>
+    <t>Fri, 14 Jun 2024 21:18:14 +0000</t>
+  </si>
+  <si>
     <t>$11.00-$40.00</t>
   </si>
   <si>
+    <t>$12.00-$36.00</t>
+  </si>
+  <si>
     <t>June 14, 2024 21:50 UTC</t>
   </si>
   <si>
+    <t>June 14, 2024 21:18 UTC</t>
+  </si>
+  <si>
     <t>Video Editing</t>
   </si>
   <si>
     <t>Video Cleanup,     Adobe Illustrator,     Adobe Photoshop,     Adobe Premiere Pro,     Instagram Reels,     Instagram Story,     Live Action Video,     Video Editing,     Testimonial Video,     Caption</t>
+  </si>
+  <si>
+    <t>DaVinci Resolve,     Video Post-Editing</t>
   </si>
   <si>
     <t>United States</t>
@@ -526,7 +594,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -596,34 +664,34 @@
         <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -635,6 +703,56 @@
         <v>0</v>
       </c>
       <c r="R2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>24</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -642,6 +760,8 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>